<commit_message>
SC : Avancement du tp5.
</commit_message>
<xml_diff>
--- a/tp5/Question 2 - Tableaux.xlsx
+++ b/tp5/Question 2 - Tableaux.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
   <si>
     <t>HIT</t>
   </si>
@@ -86,20 +86,236 @@
     <t>Ensemble de deux</t>
   </si>
   <si>
-    <t>47 | 241</t>
-  </si>
-  <si>
-    <t>12 | 455</t>
-  </si>
-  <si>
     <t>Ensemble de qautre</t>
+  </si>
+  <si>
+    <t>0x2F | 0xF1</t>
+  </si>
+  <si>
+    <t>0x2F x</t>
+  </si>
+  <si>
+    <t>0x1E x</t>
+  </si>
+  <si>
+    <t>0x34 x</t>
+  </si>
+  <si>
+    <t>0xC</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>0x65 x</t>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>0xDB</t>
+  </si>
+  <si>
+    <t>0F1</t>
+  </si>
+  <si>
+    <t>0x1C7</t>
+  </si>
+  <si>
+    <t>0xC | 0x1C7</t>
+  </si>
+  <si>
+    <t>0x46 | 0xDB</t>
+  </si>
+  <si>
+    <t>0x1E | 0xDB</t>
+  </si>
+  <si>
+    <t>0x34 | 0xDB</t>
+  </si>
+  <si>
+    <t>0x65 | 0xF1</t>
+  </si>
+  <si>
+    <t>0x1C | 0x1C7</t>
+  </si>
+  <si>
+    <t>0x5E | 0xF1</t>
+  </si>
+  <si>
+    <t>0x19 | 0xC7</t>
+  </si>
+  <si>
+    <t>0x5F | 0xF1</t>
+  </si>
+  <si>
+    <t>0x8C | 0xDB</t>
+  </si>
+  <si>
+    <t>0x3C | 0xDB</t>
+  </si>
+  <si>
+    <t>0x68 | 0xDB</t>
+  </si>
+  <si>
+    <t>0xCA | 0xF1</t>
+  </si>
+  <si>
+    <t>0x39 | 0xC7</t>
+  </si>
+  <si>
+    <t>0x5E x</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>0x8C</t>
+  </si>
+  <si>
+    <t>0x3C x</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>0xCA x</t>
+  </si>
+  <si>
+    <t>WR 0x5EF1D</t>
+  </si>
+  <si>
+    <t>WR 0x19C7C</t>
+  </si>
+  <si>
+    <t>RD 0x5EF1B</t>
+  </si>
+  <si>
+    <t>RD 0x8CDB0</t>
+  </si>
+  <si>
+    <t>WR 0x3CDB3</t>
+  </si>
+  <si>
+    <t>WR 0x5EF15</t>
+  </si>
+  <si>
+    <t>RD 0x68DBF</t>
+  </si>
+  <si>
+    <t>WR 0xCAF1C</t>
+  </si>
+  <si>
+    <t>WR 0x39C7E</t>
+  </si>
+  <si>
+    <t>RD 0xCAF1A</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>2 blocs</t>
+  </si>
+  <si>
+    <t>4 blocs</t>
+  </si>
+  <si>
+    <t>0x2F</t>
+  </si>
+  <si>
+    <t>0xF1</t>
+  </si>
+  <si>
+    <t>0x1E</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>0x65</t>
+  </si>
+  <si>
+    <t>0x5E</t>
+  </si>
+  <si>
+    <t>0xC7</t>
+  </si>
+  <si>
+    <t>0x5F</t>
+  </si>
+  <si>
+    <t>0x3C</t>
+  </si>
+  <si>
+    <t>0xCA</t>
+  </si>
+  <si>
+    <t>0x39</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>0x2F1</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0x1A</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>0x0DB</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0F1</t>
+  </si>
+  <si>
+    <t>0x034</t>
+  </si>
+  <si>
+    <t>Tag0</t>
+  </si>
+  <si>
+    <t>Tag1</t>
+  </si>
+  <si>
+    <t>Tag2</t>
+  </si>
+  <si>
+    <t>Tag3</t>
+  </si>
+  <si>
+    <t>0x32*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +330,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,7 +347,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -434,11 +658,366 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,9 +1052,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -488,26 +1064,173 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,36 +1509,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:M40"/>
+  <dimension ref="C5:AM52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="13" width="8.83203125" customWidth="1"/>
+    <col min="3" max="13" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" customWidth="1"/>
+    <col min="17" max="28" width="6.5" customWidth="1"/>
+    <col min="30" max="31" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="3:13" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="21" t="s">
+    <row r="5" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="3:39" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="Q6" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="V6" s="61"/>
+      <c r="W6" s="61"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z6" s="61"/>
+      <c r="AA6" s="61"/>
+      <c r="AB6" s="61"/>
+      <c r="AD6" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="65"/>
+      <c r="AI6" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ6" s="67"/>
+      <c r="AK6" s="67"/>
+      <c r="AL6" s="67"/>
+      <c r="AM6" s="68"/>
+    </row>
+    <row r="7" spans="3:39" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="43" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -848,45 +1608,155 @@
       <c r="M7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="17"/>
-      <c r="D8" s="18" t="s">
+      <c r="P7" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="S7" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="W7" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="X7" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z7" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA7" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB7" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE7" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF7" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG7" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH7" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI7" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ7" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK7" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL7" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM7" s="49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="3:39" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="44"/>
+      <c r="D8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="13" t="s">
+      <c r="P8" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" s="51"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="V8" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="W8" s="51"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="51"/>
+      <c r="AD8" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE8" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="69"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+    </row>
+    <row r="9" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
         <v>11</v>
@@ -902,9 +1772,50 @@
       <c r="M9" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C10" s="14" t="s">
+      <c r="P9" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="R9" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="53"/>
+      <c r="U9" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="V9" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="W9" s="5"/>
+      <c r="X9" s="53"/>
+      <c r="Y9" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z9" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AD9" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE9" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="50"/>
+      <c r="AI9" s="69"/>
+      <c r="AJ9" s="49"/>
+      <c r="AK9" s="49"/>
+      <c r="AL9" s="49"/>
+      <c r="AM9" s="49"/>
+    </row>
+    <row r="10" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C10" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="10"/>
@@ -923,9 +1834,56 @@
         <v>11</v>
       </c>
       <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C11" s="14">
+      <c r="P10" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="R10" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="53"/>
+      <c r="U10" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X10" s="53"/>
+      <c r="Y10" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z10" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB10" s="5"/>
+      <c r="AD10" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE10" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="69"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="49"/>
+    </row>
+    <row r="11" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C11" s="13">
         <v>219</v>
       </c>
       <c r="D11" s="10"/>
@@ -944,9 +1902,36 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C12" s="14">
+      <c r="P11" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="53"/>
+      <c r="U11" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="V11" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="53"/>
+      <c r="Y11" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z11" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C12" s="13">
         <v>455</v>
       </c>
       <c r="D12" s="10"/>
@@ -963,9 +1948,40 @@
         <v>14</v>
       </c>
       <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="15">
+      <c r="P12" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="R12" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="53"/>
+      <c r="U12" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="V12" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="W12" s="5"/>
+      <c r="X12" s="53"/>
+      <c r="Y12" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z12" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="14">
         <v>753</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -988,26 +2004,183 @@
       <c r="M13" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:13" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="21" t="s">
+      <c r="P13" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" s="53"/>
+      <c r="Y13" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z13" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+    </row>
+    <row r="14" spans="3:39" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="V14" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="W14" s="5"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z14" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+    </row>
+    <row r="15" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="P15" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="R15" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="U15" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="V15" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="W15" s="5"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+    </row>
+    <row r="16" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="P16" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="R16" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="5"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="V16" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="W16" s="5"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z16" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="P17" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q17" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="R17" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="53"/>
+      <c r="U17" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="V17" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z17" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB17" s="5"/>
+    </row>
+    <row r="18" spans="3:28" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="3:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="12" t="s">
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="R19" s="42"/>
+    </row>
+    <row r="20" spans="3:28" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="43" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -1041,44 +2214,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="17"/>
-      <c r="D21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="19" t="s">
+    <row r="21" spans="3:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="44"/>
+      <c r="D21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C22" s="13" t="s">
+      <c r="E21" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C22" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
         <v>11</v>
@@ -1095,8 +2268,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+    <row r="23" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C23" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="10"/>
@@ -1105,283 +2278,437 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J23" s="31"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C24" s="14">
-        <v>219</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5">
-        <v>35</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5">
+    <row r="24" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C24" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C25" s="36"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C27" s="36"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C25" s="14">
-        <v>241</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5">
-        <v>14</v>
-      </c>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="15">
-        <v>455</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="3:13" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="23"/>
-    </row>
-    <row r="33" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="12" t="s">
+      <c r="L27" s="3"/>
+      <c r="M27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C28" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="20"/>
+    </row>
+    <row r="29" spans="3:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="37"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="25"/>
+    </row>
+    <row r="30" spans="3:28" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="3:13" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="34"/>
+    </row>
+    <row r="36" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="17"/>
-      <c r="D34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L34" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C35" s="13" t="s">
+    <row r="37" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="44"/>
+      <c r="D37" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C38" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C36" s="14" t="s">
+      <c r="D38" s="15"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C39" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C37" s="14">
-        <v>219</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5">
-        <v>35</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5">
-        <v>26</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C38" s="14">
-        <v>241</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5">
-        <v>14</v>
-      </c>
-      <c r="M38" s="6"/>
-    </row>
-    <row r="39" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="15">
-        <v>455</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" s="7"/>
-      <c r="M39" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C40" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="21"/>
+      <c r="E40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="20"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C41" s="39"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="29"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C42" s="39"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="29"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C43" s="40"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C44" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="29"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C45" s="39"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="29"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C46" s="39"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="29"/>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C47" s="40"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C48" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="29"/>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C49" s="39"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="L49" s="28"/>
+      <c r="M49" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C50" s="39"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="29"/>
+    </row>
+    <row r="51" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="41"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="25"/>
+    </row>
+    <row r="52" spans="3:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C33:C34"/>
+  <mergeCells count="18">
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AF6:AH6"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C6:M6"/>
     <mergeCell ref="C19:M19"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C32:M32"/>
+    <mergeCell ref="C35:M35"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>